<commit_message>
Made changes to prio list
</commit_message>
<xml_diff>
--- a/Projektplanering/Projektuppgift YSYS-OP1 2020-10-20.xlsx
+++ b/Projektplanering/Projektuppgift YSYS-OP1 2020-10-20.xlsx
@@ -18,7 +18,7 @@
     <sheet name="Ytterligare Krav" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Ytterligare Krav'!$A$12:$D$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Ytterligare Krav'!$A$12:$E$12</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="109">
   <si>
     <t>Vad ska ni göra?</t>
   </si>
@@ -361,13 +361,29 @@
   <si>
     <t>•  Kravens prioritet, förtydligande detaljer och den totala omfattningen 
      (vilka krav som ska implementeras) av Release 2 ska dokumenteras i rapporten.</t>
+  </si>
+  <si>
+    <t>Måste detta vara en ny Vy eller kan man utöka befintlig</t>
+  </si>
+  <si>
+    <t>Vad betyder detta. Alla kund ordrar eller leverantörs ordrar eller alla ordrar</t>
+  </si>
+  <si>
+    <t>Vad betyder detta. Att man ska kunna beställa mot leverantör. 
+Måste detta vara en ny Vy eller kan man utöka befintlig</t>
+  </si>
+  <si>
+    <t>Kommentarer</t>
+  </si>
+  <si>
+    <t>Vad för info ska finnas om för online kunder och är det två kundlistor man ska ha eller en.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -379,6 +395,12 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -404,18 +426,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -429,6 +441,18 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,7 +745,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -741,7 +765,7 @@
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -761,17 +785,17 @@
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -781,22 +805,22 @@
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
+      <c r="A24" s="2"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -809,12 +833,12 @@
       </c>
     </row>
     <row r="29" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -824,12 +848,12 @@
       </c>
     </row>
     <row r="32" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -844,7 +868,7 @@
       </c>
     </row>
     <row r="39" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -854,7 +878,7 @@
       </c>
     </row>
     <row r="41" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -883,7 +907,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -893,7 +917,7 @@
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -908,12 +932,12 @@
       </c>
     </row>
     <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -928,22 +952,22 @@
       </c>
     </row>
     <row r="12" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -967,7 +991,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -992,7 +1016,7 @@
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1022,7 +1046,7 @@
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1057,12 +1081,12 @@
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1082,7 +1106,7 @@
       </c>
     </row>
     <row r="33" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1112,7 +1136,7 @@
       </c>
     </row>
     <row r="41" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="1" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1122,7 +1146,7 @@
       </c>
     </row>
     <row r="43" spans="1:1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="2" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1132,7 +1156,7 @@
       </c>
     </row>
     <row r="45" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1146,426 +1170,443 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.42578125" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="73.7109375" customWidth="1"/>
+    <col min="5" max="5" width="107.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="4" t="s">
         <v>79</v>
       </c>
+      <c r="E12" s="4" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="5">
         <v>1</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5">
+        <v>2</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>3</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5">
+        <v>3</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>4</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5">
+        <v>6</v>
+      </c>
+      <c r="D16" s="13" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>2</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5">
+        <v>7</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>6</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5">
+        <v>8</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>7</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5">
+        <v>9</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
-        <v>3</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E19" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>8</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5">
+        <v>10</v>
+      </c>
+      <c r="D20" s="13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>9</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5">
+        <v>12</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>10</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5">
+        <v>13</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>11</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5">
+        <v>14</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>12</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5">
+        <v>15</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>13</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5">
         <v>4</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9">
+      <c r="D25" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>14</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5">
         <v>5</v>
       </c>
-      <c r="D16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>5</v>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
-        <v>6</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9">
+      <c r="D26" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
         <v>15</v>
       </c>
-      <c r="D18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
-        <v>7</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9">
-        <v>3</v>
-      </c>
-      <c r="D19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
-        <v>8</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
-        <v>9</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
-        <v>10</v>
-      </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9">
-        <v>9</v>
-      </c>
-      <c r="D22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>16</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5">
+        <v>17</v>
+      </c>
+      <c r="D28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>17</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5">
         <v>11</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9">
-        <v>10</v>
-      </c>
-      <c r="D23" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
-        <v>12</v>
-      </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9">
-        <v>11</v>
-      </c>
-      <c r="D24" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
-        <v>13</v>
-      </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9">
-        <v>17</v>
-      </c>
-      <c r="D25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
-        <v>14</v>
-      </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9">
-        <v>18</v>
-      </c>
-      <c r="D26" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
-        <v>15</v>
-      </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9">
-        <v>12</v>
-      </c>
-      <c r="D27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
-        <v>16</v>
-      </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9">
-        <v>13</v>
-      </c>
-      <c r="D28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
-        <v>17</v>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9">
-        <v>16</v>
       </c>
       <c r="D29" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+      <c r="E29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
         <v>18</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9">
-        <v>14</v>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5">
+        <v>18</v>
       </c>
       <c r="D30" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
+      <c r="A33" s="7"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
+      <c r="A34" s="7"/>
     </row>
     <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
     </row>
     <row r="39" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A12:D30">
-    <sortState ref="A13:D30">
-      <sortCondition ref="A13:A30"/>
+  <autoFilter ref="A12:E12">
+    <sortState ref="A13:E30">
+      <sortCondition ref="A12"/>
     </sortState>
   </autoFilter>
   <mergeCells count="11">
@@ -1582,6 +1623,6 @@
     <mergeCell ref="A8:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes to Prio list after meeting with PO
</commit_message>
<xml_diff>
--- a/Projektplanering/Projektuppgift YSYS-OP1 2020-10-20.xlsx
+++ b/Projektplanering/Projektuppgift YSYS-OP1 2020-10-20.xlsx
@@ -442,17 +442,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1170,8 +1170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,74 +1188,74 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1287,7 +1287,7 @@
       <c r="C13" s="5">
         <v>1</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1299,7 +1299,7 @@
       <c r="C14" s="5">
         <v>2</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="9" t="s">
         <v>87</v>
       </c>
       <c r="E14" t="s">
@@ -1314,185 +1314,185 @@
       <c r="C15" s="5">
         <v>3</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="9" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5">
-        <v>6</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" t="s">
-        <v>104</v>
+        <v>4</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5">
-        <v>7</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>83</v>
+        <v>5</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5">
-        <v>8</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>84</v>
+        <v>6</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5">
-        <v>9</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>106</v>
+        <v>7</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5">
-        <v>10</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>82</v>
+        <v>8</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5">
-        <v>12</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>85</v>
+        <v>9</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5">
-        <v>13</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>89</v>
+        <v>10</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5">
-        <v>14</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>90</v>
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5">
-        <v>15</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>91</v>
+        <v>12</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5">
-        <v>4</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>94</v>
+        <v>13</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5">
-        <v>5</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>95</v>
+        <v>14</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5">
-        <v>16</v>
-      </c>
-      <c r="D27" t="s">
-        <v>92</v>
+        <v>15</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>96</v>
-      </c>
-      <c r="E29" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1520,107 +1520,107 @@
       <c r="A34" s="7"/>
     </row>
     <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
     </row>
     <row r="39" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A12:E12">
     <sortState ref="A13:E30">
-      <sortCondition ref="A12"/>
+      <sortCondition ref="C12"/>
     </sortState>
   </autoFilter>
   <mergeCells count="11">
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A7:J7"/>
+    <mergeCell ref="A8:J8"/>
     <mergeCell ref="A40:J40"/>
     <mergeCell ref="A35:J35"/>
     <mergeCell ref="A36:J36"/>
     <mergeCell ref="A37:J37"/>
     <mergeCell ref="A38:J38"/>
     <mergeCell ref="A39:J39"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A7:J7"/>
-    <mergeCell ref="A8:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>